<commit_message>
LuanNT bao cao, tao xong cac tables CSDL
</commit_message>
<xml_diff>
--- a/Prj_ERROR404/00_Documents/BangChamCong.xlsx
+++ b/Prj_ERROR404/00_Documents/BangChamCong.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Nội dung</t>
   </si>
@@ -103,6 +103,11 @@
     <t>*Hoàn thành phân tích yêu cầu CSDL, Chức năng hệ thống:
 \02_Member\LuanNT\20140907_DatabaseDesign\YeuCauCSDL.xlsx
 *Todo: các chức năng admin, users, clients</t>
+  </si>
+  <si>
+    <t>*Hoàn thành thiết kế CSDL cơ bản (bảng author,book,user…)
+\02_Member\LuanNT\20140911_DatabaseDesign\CSDL.xlsx
+*Todo: mô hình thực thể liên kết, View, Funtions…</t>
   </si>
 </sst>
 </file>
@@ -543,7 +548,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -709,6 +714,17 @@
       </c>
       <c r="I8" s="15" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45">
+      <c r="C9" s="3">
+        <v>41952</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="7:7">

</xml_diff>

<commit_message>
LuanNT commit Hop du an
</commit_message>
<xml_diff>
--- a/Prj_ERROR404/00_Documents/BangChamCong.xlsx
+++ b/Prj_ERROR404/00_Documents/BangChamCong.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Nội dung</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t>17/9/2014</t>
+  </si>
+  <si>
+    <t>*Tổng hợp kiến thức cá nhân mỗi người
+*Kế hoạch tiếp theo</t>
+  </si>
+  <si>
+    <t>Xác nhận mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Tìm hiểu xác nhận mail đăng nhập
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+*Todo: Tìm hiểu về cơ chế sinh link, key để đăng ký acc cho website</t>
+  </si>
+  <si>
+    <t>27/9/2014</t>
   </si>
 </sst>
 </file>
@@ -587,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,7 +846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -842,28 +860,82 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="14"/>
+      <c r="F24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:11">
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:11">
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:11">
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:11">
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:11">
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:11">
       <c r="G31" s="16"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:11">
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="7:7">

</xml_diff>